<commit_message>
Update - After 100m (Male)
</commit_message>
<xml_diff>
--- a/SCRC_2024_Olympics_Pool_PICKS.xlsx
+++ b/SCRC_2024_Olympics_Pool_PICKS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noahc\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/67bd65b767a0c66b/Documents/SCRC Olympics PICKS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A67B3BB-423D-43DE-9027-BA74F36415DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="8_{D84A91DA-60D3-4F5D-ACEB-AB2123FA66D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E30DF36E-12BC-4DC6-AFE0-B3FFB98D44AB}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2865" yWindow="4215" windowWidth="25935" windowHeight="11385" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ALL_ENTRIES" sheetId="5" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="63">
   <si>
     <t>Event</t>
   </si>
@@ -216,24 +216,6 @@
   </si>
   <si>
     <t>4x100m - F</t>
-  </si>
-  <si>
-    <t>Andre De-Grasse</t>
-  </si>
-  <si>
-    <t>Shelley-Ann Fraser-Pryce</t>
-  </si>
-  <si>
-    <t>Zhamel Hughes</t>
-  </si>
-  <si>
-    <t>Alexander Doom</t>
-  </si>
-  <si>
-    <t>Marliedy Paulino</t>
-  </si>
-  <si>
-    <t>Natasha Pryce</t>
   </si>
 </sst>
 </file>
@@ -596,6 +578,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
@@ -883,10 +869,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFA354F7-B6AD-4E14-AF45-3439114430B4}">
-  <dimension ref="A1:E69"/>
+  <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="D63" sqref="D63"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -895,7 +881,7 @@
     <col min="2" max="2" width="19.5703125" style="24" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.7109375" style="24" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.7109375" style="24" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7" style="24" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6" style="24" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="18.85546875" style="24"/>
   </cols>
   <sheetData>
@@ -1726,147 +1712,8 @@
       </c>
       <c r="E59" s="27"/>
     </row>
-    <row r="60" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="61" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B61" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C61" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="D61" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="E61" s="17"/>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A62" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="B62" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C62" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="D62" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="E62" s="25" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A63" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="B63" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="C63" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="D63" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="E63" s="26"/>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A64" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="B64" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C64" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="D64" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="E64" s="26"/>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A65" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="B65" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="C65" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="D65" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="E65" s="26"/>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A66" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="B66" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="C66" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="D66" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="E66" s="26"/>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A67" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="B67" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="C67" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="D67" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="E67" s="26"/>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A68" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="B68" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="C68" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="D68" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="E68" s="26"/>
-    </row>
-    <row r="69" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="B69" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="C69" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="D69" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="E69" s="27"/>
-    </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="E62:E69"/>
+  <mergeCells count="6">
     <mergeCell ref="E52:E59"/>
     <mergeCell ref="E2:E9"/>
     <mergeCell ref="E12:E19"/>
@@ -2876,17 +2723,17 @@
   </sheetPr>
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.3">
@@ -2908,15 +2755,9 @@
       <c r="A2" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>63</v>
-      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="8"/>
       <c r="E2" s="28" t="s">
         <v>53</v>
       </c>
@@ -2925,105 +2766,63 @@
       <c r="A3" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>19</v>
-      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="8"/>
       <c r="E3" s="29"/>
     </row>
     <row r="4" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>65</v>
-      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="8"/>
       <c r="E4" s="29"/>
     </row>
     <row r="5" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>21</v>
-      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="8"/>
       <c r="E5" s="29"/>
     </row>
     <row r="6" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>27</v>
-      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="8"/>
       <c r="E6" s="29"/>
     </row>
     <row r="7" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>41</v>
-      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="8"/>
       <c r="E7" s="29"/>
     </row>
     <row r="8" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>32</v>
-      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="8"/>
       <c r="E8" s="29"/>
     </row>
     <row r="9" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="B9" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>42</v>
-      </c>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="11"/>
       <c r="E9" s="30"/>
     </row>
   </sheetData>

</xml_diff>